<commit_message>
new influence and sensitivity metrics, add table
</commit_message>
<xml_diff>
--- a/parameter_files/base/de_dg_gw_upper.xlsx
+++ b/parameter_files/base/de_dg_gw_upper.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25330"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25928"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/4efc3e9dc81381f4/Documents/SJV-gen-modeling/parameter_files/base/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="12" documentId="8_{027CEFEE-6977-4EF3-9714-F9BE2629FBB8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7227F2C8-D410-4EE1-8AF0-97F5477C08B4}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="106_{460627E5-9D15-4BAA-8D6D-D9B571D28BEC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{79620C5E-93EC-41E4-B7D2-2730489730D1}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{79620C5E-93EC-41E4-B7D2-2730489730D1}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -652,7 +652,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme 2013 - 2022" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>

</xml_diff>